<commit_message>
agregando el consolidado de ricardito
</commit_message>
<xml_diff>
--- a/EDER_GOMEZ_4TO_BIMESTRE_PRIMERO_SECUNDARIA.xlsx
+++ b/EDER_GOMEZ_4TO_BIMESTRE_PRIMERO_SECUNDARIA.xlsx
@@ -1416,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DL56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4242,9 +4242,7 @@
       <c r="K12" s="3">
         <v>16</v>
       </c>
-      <c r="L12" s="3">
-        <v>15</v>
-      </c>
+      <c r="L12" s="3"/>
       <c r="M12" s="3">
         <v>16</v>
       </c>
@@ -4254,9 +4252,7 @@
       <c r="O12" s="3">
         <v>16</v>
       </c>
-      <c r="P12" s="3">
-        <v>15</v>
-      </c>
+      <c r="P12" s="3"/>
       <c r="Q12" s="3">
         <v>14</v>
       </c>
@@ -7844,9 +7840,7 @@
       <c r="K26" s="3">
         <v>17</v>
       </c>
-      <c r="L26" s="3">
-        <v>15</v>
-      </c>
+      <c r="L26" s="3"/>
       <c r="M26" s="3">
         <v>17</v>
       </c>
@@ -7856,9 +7850,7 @@
       <c r="O26" s="3">
         <v>17</v>
       </c>
-      <c r="P26" s="3">
-        <v>15</v>
-      </c>
+      <c r="P26" s="3"/>
       <c r="Q26" s="3">
         <v>16</v>
       </c>
@@ -13708,9 +13700,7 @@
       <c r="K49" s="3">
         <v>15</v>
       </c>
-      <c r="L49" s="3">
-        <v>14</v>
-      </c>
+      <c r="L49" s="3"/>
       <c r="M49" s="3">
         <v>16</v>
       </c>
@@ -13720,9 +13710,7 @@
       <c r="O49" s="3">
         <v>15</v>
       </c>
-      <c r="P49" s="3">
-        <v>14</v>
-      </c>
+      <c r="P49" s="3"/>
       <c r="Q49" s="3">
         <v>13</v>
       </c>

</xml_diff>